<commit_message>
returning url and stopwords
</commit_message>
<xml_diff>
--- a/app_reviews/outputs/result.xlsx
+++ b/app_reviews/outputs/result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="205">
   <si>
     <t>reviewer_name</t>
   </si>
@@ -38,10 +38,28 @@
     <t>new</t>
   </si>
   <si>
-    <t>Sagar Raj</t>
-  </si>
-  <si>
-    <t>11 March 2019</t>
+    <t>Nicosius Geraldi</t>
+  </si>
+  <si>
+    <t>March 13, 2019</t>
+  </si>
+  <si>
+    <t>Rated 1 stars out of five stars</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>semua secara tokopedia z button toko yg gini renggut dipilih hanya ini tidak customer untuk dengan hak sebagai tapi durasi di sudah sesuai mau update sampai pengiriman versi ada kaya semenjak apps apa terbaru tulisan kurir otomatis dan layanan saya memilih maksudnya bisa inginkan preferensi pilih</t>
+  </si>
+  <si>
+    <t>semua secara tokopedia z button toko yg gini renggut dipilih hanya ini tidak customer untuk dengan hak sebagai tapi durasi di sudah sesuai mau update sampai pengiriman versi ada kaya semenjak  apa terbaru tulisan kurir otomatis dan layanan saya memilih maksudnya bisa inginkan preferensi pilih</t>
+  </si>
+  <si>
+    <t>patrick wong</t>
   </si>
   <si>
     <t>Rated 2 stars out of five stars</t>
@@ -50,679 +68,568 @@
     <t>2</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>hazard best tests pressure way bot wallets also finding bypass payment great high heart claims luck risk although seemingly susceptible digibank chat virtual extent blood real health incentives patience using attacks</t>
-  </si>
-  <si>
-    <t>hazard best tests pressure way bot wallets also finding bypass payment great high heart claims luck risk although seemingly susceptible  chat virtual extent blood real health incentives patience using attacks</t>
-  </si>
-  <si>
-    <t>VINAYAK KADAM</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>dan menu faq bantuan tidak berfungsi</t>
+  </si>
+  <si>
+    <t>Mares Pradana</t>
+  </si>
+  <si>
+    <t>Rated 5 stars out of five stars</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>aplikasi dapat dan loading terima pemakaian setelah berjalan saya lancar langsung komplain awal tanggapan kasih lambat sangat</t>
+  </si>
+  <si>
+    <t>Hadi Wibowo</t>
+  </si>
+  <si>
+    <t>March 12, 2019</t>
+  </si>
+  <si>
+    <t>masuk banyak dng abal tawarkan gak sayang yg mulai murahnya harga belanja akalmencurigakan mudah penjual barang</t>
+  </si>
+  <si>
+    <t>A Google user</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>ga ligat riwayat update transaksi bisa habis di</t>
+  </si>
+  <si>
+    <t>Zeth ImmanueL Tendean Jr</t>
+  </si>
+  <si>
+    <t>aplikasi ga nya ada mati</t>
+  </si>
+  <si>
+    <t>pietro Hardi</t>
+  </si>
+  <si>
+    <t>bagus marketpalce ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bagus marketpalce </t>
+  </si>
+  <si>
+    <t>Edgina Rahma</t>
+  </si>
+  <si>
+    <t>keep working dude apps great good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keep working dude  great </t>
+  </si>
+  <si>
+    <t>Muhammad Harun</t>
+  </si>
+  <si>
+    <t>membantu dan app excellent sangat</t>
+  </si>
+  <si>
+    <t>membantu dan  excellent sangat</t>
+  </si>
+  <si>
+    <t>Lex Bong</t>
+  </si>
+  <si>
+    <t>March 11, 2019</t>
+  </si>
+  <si>
+    <t>keren toped</t>
+  </si>
+  <si>
+    <t>Terry Aja</t>
+  </si>
+  <si>
+    <t>aplikasi mantab</t>
+  </si>
+  <si>
+    <t>Ira Yuska</t>
+  </si>
+  <si>
+    <t>application good</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Alfian Nur Sya'bana</t>
+  </si>
+  <si>
+    <t>trash</t>
+  </si>
+  <si>
+    <t>Fauzy Nadjar</t>
+  </si>
+  <si>
+    <t>good app</t>
+  </si>
+  <si>
+    <t>Muhammad Muslimin Ikbal</t>
+  </si>
+  <si>
+    <t>terpercaya good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terpercaya </t>
+  </si>
+  <si>
+    <t>nico wijaya</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>Irwan Chai</t>
+  </si>
+  <si>
+    <t>March 6, 2019</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>saatnya parah ke malah history tau tambah caranya timeout terus aplikasi ga mau update gw lain trus ulasan makin hijrah baik aja saya pembelian cara nulis bukannya liat</t>
+  </si>
+  <si>
+    <t>Paul Asido</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>pesan diskusi ketika mau parah update saya banned malah sbg user kurang zzzz isi muncul terakhir lebih produk error</t>
+  </si>
+  <si>
+    <t>Hendry Utama</t>
+  </si>
+  <si>
+    <t>March 4, 2019</t>
   </si>
   <si>
     <t>Rated 3 stars out of five stars</t>
   </si>
   <si>
-    <t>3</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>ditawarkan ongkir hilang yg diganti kurang sejak ini tidak memang des dibanding lainnya lbh perbulan utk menarik kupon pakai program lagi 8 undian2 karena bagus official free jelas didukung dan banyak store nilainya promo 2019 ovo kecil cashback maret 2018 awal jadi</t>
+  </si>
+  <si>
+    <t>March 7, 2019</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>shown smoothly hectic reacharge make want recharge otherwise amount concept times app list oh says error improve plan using valid nice enter things many trying</t>
-  </si>
-  <si>
-    <t>shown smoothly hectic reacharge make want recharge otherwise amount concept times  list oh says error improve plan using valid nice enter things many trying</t>
-  </si>
-  <si>
-    <t>Arun Saxena</t>
-  </si>
-  <si>
-    <t>4 March 2019</t>
-  </si>
-  <si>
-    <t>Rated 5 stars out of five stars</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>fingerfrint thanks unable working wrong 4 reset times details app account needs login password upgrade complete shows dbs always scanning fine mu</t>
-  </si>
-  <si>
-    <t>fingerfrint thanks unable working wrong 4 reset times details  account needs login password upgrade complete shows  always scanning fine mu</t>
-  </si>
-  <si>
-    <t>ashish athalye</t>
-  </si>
-  <si>
-    <t>10 March 2019</t>
-  </si>
-  <si>
-    <t>self fees also kindly withdrawls mumbai app limit trouble update location mentioned navimumbai withdrawl lot done free mention placed atm logging charging dbs heavy stipulated gives transaction</t>
-  </si>
-  <si>
-    <t>self fees also kindly withdrawls mumbai  limit trouble update location mentioned navimumbai withdrawl lot done free mention placed atm logging charging  heavy stipulated gives transaction</t>
-  </si>
-  <si>
-    <t>Benson Gomez</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>clear memory completely close background slow compared app everytime recent banking button exist apps</t>
-  </si>
-  <si>
-    <t>clear memory completely close background slow compared  everytime recent  button exist apps</t>
-  </si>
-  <si>
-    <t>Teeds Chauhan</t>
-  </si>
-  <si>
-    <t>6 March 2019</t>
+    <t>ga tokopedia juga snk worst cs ever sangat langgar malah cashback real tapi pelayanan payah marketplace dibatalkan di order</t>
+  </si>
+  <si>
+    <t>Chris Fransiska</t>
+  </si>
+  <si>
+    <t>March 5, 2019</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>ya dicurangin tertera ui bs kecurangan check hilang checkout banget klo toped coba kalau meskipun input bayar tapi aneh sebelum belum di jd blm ga kupon halaman donk lagi poor mau rugi update tp gw atau masuk cek sy cashback bisa korban invoice udah sehingga akrg</t>
+  </si>
+  <si>
+    <t>Dedi Andika</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>kenapa dan seharusnya informasi buka tiket lainlain tolong diperbaiki saya dalam pesawat bugnya yg bisa tak notifikasi muncul ditampilkan</t>
+  </si>
+  <si>
+    <t>Ashar Sulaksono</t>
+  </si>
+  <si>
+    <t>March 10, 2019</t>
+  </si>
+  <si>
+    <t>kupon pakai susah menu ovo gak history point dicari bisa dipake belanja</t>
+  </si>
+  <si>
+    <t>Ferdy Karler</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>registered upi unavailable number later want 10 times app registering server show money register time end many asking charging try already charge 150rs</t>
-  </si>
-  <si>
-    <t>registered upi unavailable number later want 10 times  registering server show money register time end many asking charging try already charge 150rs</t>
-  </si>
-  <si>
-    <t>Mrityunjaya Paniquar</t>
-  </si>
-  <si>
-    <t>9 March 2019</t>
+    <t>ga blunder selesaiin pdhl transaksi sampe bisa paket udah jadi</t>
+  </si>
+  <si>
+    <t>MD Raditya</t>
+  </si>
+  <si>
+    <t>bingung menu kadang bikin update keluar kadah malah history kagak belanja dimana</t>
+  </si>
+  <si>
+    <t>Rivandanu Fadhli</t>
   </si>
   <si>
     <t>Rated 4 stars out of five stars</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>later difficulty great however whims updates app one ever initially digibank swidt card wnjoying promotions well featurea beilliant oblige dbs year many faored</t>
-  </si>
-  <si>
-    <t>later difficulty great however whims updates  one ever initially  swidt card wnjoying promotions well featurea beilliant oblige  year many faored</t>
-  </si>
-  <si>
-    <t>Neel Sarkar</t>
-  </si>
-  <si>
-    <t>Rated 1 stars out of five stars</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>spend get denied 1000 offer diwali claimed spender iphone said give 20000 top</t>
-  </si>
-  <si>
-    <t>A Google user</t>
-  </si>
-  <si>
-    <t>works pop fingerprint complete properly update thr buggy need app also biometric verification going still completed login</t>
-  </si>
-  <si>
-    <t>works pop fingerprint complete properly update thr buggy need  also biometric verification going still completed login</t>
-  </si>
-  <si>
-    <t>Akbar Barbhuiya</t>
-  </si>
-  <si>
-    <t>13 March 2019</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>irritated bank thousand withdrewn low 10000 month also balance maximum 10 appropriate iti withdrawal user joke cant anither plz jokes per k enough 10k dbs system day deposit rectify</t>
-  </si>
-  <si>
-    <t>irritated  thousand withdrewn low 10000 month also balance maximum 10 appropriate iti withdrawal user joke cant anither plz jokes per k enough 10k  system day deposit rectify</t>
-  </si>
-  <si>
-    <t>Prantik Sarkar</t>
+    <t>itu tidak menjadi penanganan setelah 13 handphone berubah nomor jumlah saat bila sudah kolom ubah ditulis review 08xxx ada pula thanks digit nya otomatis dan diedit akan karna 628xxx saya transaksi bisa awal jadi disave</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>dapat penipuan ternyata buka toko promoke hpbiar orang buat pedia setiap aplikasinya memancing</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>tokopedia banyak diskon dan ongkir parah saja dengan kecewa gratis malah tambah bener bukannya maret ini awal</t>
+  </si>
+  <si>
+    <t>darmadi chandra</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>bengek diskusi dan belasan kolom lihatnya padahal click follow trs blink itu kali di sdh</t>
+  </si>
+  <si>
+    <t>Degi Rizcky</t>
+  </si>
+  <si>
+    <t>doang komplaint mau server tp statusnya bermasalah yg ada jawab robot terus barang chat fitu</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>last copy updatega bisa invoice</t>
+  </si>
+  <si>
+    <t>edy santosa</t>
+  </si>
+  <si>
+    <t>banyak ngak bikin punya saja jgn gan kecewa ada sortir penjual barang di dipajang</t>
+  </si>
+  <si>
+    <t>aplikasi dan sesuai diterima untuk gunakan dengan yang jual mudah barang di</t>
+  </si>
+  <si>
+    <t>studio production</t>
+  </si>
+  <si>
+    <t>lah ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lah </t>
+  </si>
+  <si>
+    <t>trims tokped</t>
+  </si>
+  <si>
+    <t>Yos Riyadi</t>
+  </si>
+  <si>
+    <t>akan tokopedia professional terjang bangga lebih sepak</t>
+  </si>
+  <si>
+    <t>Petak rumah</t>
+  </si>
+  <si>
+    <t>aplikasi perbaiki tolong segera notifikasi muncul tidak di</t>
+  </si>
+  <si>
+    <t>Marliyanti Kristy</t>
+  </si>
+  <si>
+    <t>gbsa aplikasinya buka</t>
+  </si>
+  <si>
+    <t>Sylphers Hery</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>24rb korupsi kooperatif aja ongkir parah tidak di</t>
+  </si>
+  <si>
+    <t>Adi Supranoto</t>
+  </si>
+  <si>
+    <t>March 9, 2019</t>
+  </si>
+  <si>
+    <t>tokopedia love txx33 eerf r ef rrrer f</t>
+  </si>
+  <si>
+    <t>Eric Tjan</t>
+  </si>
+  <si>
+    <t>March 8, 2019</t>
+  </si>
+  <si>
+    <t>helpful good n</t>
+  </si>
+  <si>
+    <t>helpful  n</t>
+  </si>
+  <si>
+    <t>mantab</t>
+  </si>
+  <si>
+    <t>Agung Maehendra</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>nyaman dsni belanja</t>
+  </si>
+  <si>
+    <t>good job</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> job</t>
+  </si>
+  <si>
+    <t>Dharmawan Zakky</t>
+  </si>
+  <si>
+    <t>awesome</t>
+  </si>
+  <si>
+    <t>Herald Sinaga</t>
+  </si>
+  <si>
+    <t>agus sugiharto</t>
+  </si>
+  <si>
+    <t>apps good</t>
+  </si>
+  <si>
+    <t>Dicky Saputra</t>
+  </si>
+  <si>
+    <t>great apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">great </t>
+  </si>
+  <si>
+    <t>lauren hartawan</t>
+  </si>
+  <si>
+    <t>tumbs good app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tumbs  </t>
+  </si>
+  <si>
+    <t>Luthfi Hasan</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>okelah</t>
+  </si>
+  <si>
+    <t>rahmat budi</t>
+  </si>
+  <si>
+    <t>Anthony Gunawan</t>
+  </si>
+  <si>
+    <t>Himawan Agung</t>
+  </si>
+  <si>
+    <t>mahadewa online</t>
+  </si>
+  <si>
+    <t>endang suryanendi</t>
+  </si>
+  <si>
+    <t>March 3, 2019</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>severely go least actually backandforth always even feed app soso rechecking ive tried still refreshing areas version say theres pages annoying new exists icon badge</t>
+  </si>
+  <si>
+    <t>severely go least actually backandforth always even feed  soso rechecking ive tried still refreshing areas version say theres pages annoying new exists icon badge</t>
+  </si>
+  <si>
+    <t>tokopedia bs pake terus klo error ongkirnya aplikasi connected gitu kesalahan tapi mtokopedia ga kupon server gratis aplikasinya kan kenapa via bisa maret melalui</t>
+  </si>
+  <si>
+    <t>Riza Edwin Kurniawan</t>
+  </si>
+  <si>
+    <t>March 2, 2019</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>malah error bingung app agak barang power jd ga update tiap ulasan rating ngasih via bisa house nulis buat stlh upload terakhir</t>
+  </si>
+  <si>
+    <t>malah error bingung  agak barang power jd ga update tiap ulasan rating ngasih via bisa house nulis buat stlh upload terakhir</t>
+  </si>
+  <si>
+    <t>CRB Suara Pembaruan - Memihak Kebenaran</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>semua tokopedia ongkir tadinya parah toko diganti februari ongkos pelit untuk 4 mfull kali 20 di power kirim 15 gratis yang ribu bulan 8 per gojek makin grab stok banyak 2019 khusus rp harga maret sama 5 cuman review badge semakin</t>
+  </si>
+  <si>
+    <t>do2 exe</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>notification mailbox 2019 previous bugs update quite lots spams gives februari another 29 stable ads addressed</t>
+  </si>
+  <si>
+    <t>Atmo suryo</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>lag sering dari yg bukan oenilaian repot dulunya sekarang 1 tidak produk muncul page setfull sale alasan untuk pasar quality issue jika tapi agak review 3 status buyer dg ada per terserap notifikasi membantu akan dan baik dapat 2019 flash 2 maret pengecekan seller sangat</t>
+  </si>
+  <si>
+    <t>Harris Dadlani</t>
+  </si>
+  <si>
+    <t>decreiving sure reliable money complains mske measurement quality standard back plus source buyer items gaurantee bought article good knows</t>
+  </si>
+  <si>
+    <t>decreiving sure reliable money complains mske measurement quality standard back plus source buyer items gaurantee bought article  knows</t>
+  </si>
+  <si>
+    <t>Fience Gerald</t>
+  </si>
+  <si>
+    <t>February 28, 2019</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>semua screen tokopedia dikira android kfull working emas muncul terus seamless black sebelum reksa dana transitionnya tokopoints buka update statusnya pengiriman gak status sampe hang stopped juga lambat sekitar ovo saya sama nearly review</t>
+  </si>
+  <si>
+    <t>terima muncul tidak error berhasil tanpa jika gambar kasih beserta mengirim server update 3221 versi terkirim beri terbaru ulasan keterangan akan diulas</t>
+  </si>
+  <si>
+    <t>Munawar Haris</t>
+  </si>
+  <si>
+    <t>aplikasi terusmohon tokopedia dan gangguan sebelumnya pada servernya seperti diperbaiki yang mah dulu skrang bagus deh lebih kayaknya error</t>
+  </si>
+  <si>
+    <t>Andi Hediawan</t>
+  </si>
+  <si>
+    <t>ruginyafull check mslhtolong pembelimau bannedknpapa gk lancartdk akun error bnyk aplikasi diskusi tanya laingk symsh tnyata di sperti kolom review talk insert ada apa brg artinya ituapakah jawabannyakl bsjwbannya masalah sytrakhir sy tdk user salah buat banned tokped order</t>
+  </si>
+  <si>
+    <t>Melisa Angelina</t>
+  </si>
+  <si>
+    <t>game sering ui yg crash molo terus bingung menu captain biasa sudah digunakan marvelnya bagus lokasi2 perubahan banyak cuma appsnya jadi</t>
+  </si>
+  <si>
+    <t>Johandy Huang</t>
+  </si>
+  <si>
+    <t>tokopedia telepon driver pake kurang dpt tidak chat customer aplikasi points kerjasama ujung2nfull jg dengan harus ketik better wasting mau kirim tp sayang gojek usah ada sangat2 efektif time lain brg bagus service nya dan susah spt marketplace2 reward melalui review sangat</t>
+  </si>
+  <si>
+    <t>Aileen A</t>
+  </si>
+  <si>
+    <t>cant forcing tokopedia previous spams kept back please go promoi stop sites truly irritating site pop press</t>
+  </si>
+  <si>
+    <t>李光輝suwarjono</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>best better masses need developers make tech integration basis interface microfinance providing bankinggood experienceespecially user one standardthe users awareness platform keep improving guide security savvy going</t>
-  </si>
-  <si>
-    <t>Pranjal Gupta</t>
-  </si>
-  <si>
-    <t>perfectlyits 10 interface times sluggish working ok transitionsupi 7 laggy</t>
-  </si>
-  <si>
-    <t>Jaspreet Singh</t>
-  </si>
-  <si>
-    <t>12 March 2019</t>
-  </si>
-  <si>
-    <t>drop bother chat pathetic worst even app dont revert message customer support</t>
-  </si>
-  <si>
-    <t>drop bother chat pathetic worst even  dont revert message customer support</t>
-  </si>
-  <si>
-    <t>tingku sapam</t>
-  </si>
-  <si>
-    <t>rated workingplease problem stopped low app take sson kindly action possibledeveloper fix</t>
-  </si>
-  <si>
-    <t>rated workingplease problem stopped low  take sson kindly action possibledeveloper fix</t>
-  </si>
-  <si>
-    <t>7 March 2019</t>
-  </si>
-  <si>
-    <t>window plz opens pop tells theres n problem register every create try account time later cant help</t>
-  </si>
-  <si>
-    <t>design thing make changing jo fill vahi dikta app premium happy reliable years card give using nice coustomer last debit bikta 3</t>
-  </si>
-  <si>
-    <t>design thing make changing jo fill vahi dikta  premium happy reliable years card give using nice coustomer last debit bikta 3</t>
-  </si>
-  <si>
-    <t>Sourajeet Roy</t>
-  </si>
-  <si>
-    <t>8 March 2019</t>
-  </si>
-  <si>
-    <t>necessary much slow like every fast app irritating ratings make disgusting ir ask smooth apps login</t>
-  </si>
-  <si>
-    <t>necessary much slow like every fast  irritating ratings make disgusting ir ask smooth apps login</t>
-  </si>
-  <si>
-    <t>Dinesh Kumar</t>
-  </si>
-  <si>
-    <t>could enter card pin set unable activate tried debit received proceed button diabled help please</t>
-  </si>
-  <si>
-    <t>Subham Kumar</t>
-  </si>
-  <si>
-    <t>start initial charges rs bank upto every 5 charging withdrawal without stage onwards expected withdraw unlimited happy 24 phenomenon</t>
-  </si>
-  <si>
-    <t>start initial charges rs  upto every 5 charging withdrawal without stage onwards expected withdraw unlimited happy 24 phenomenon</t>
-  </si>
-  <si>
-    <t>ACHAR NAHUSH</t>
-  </si>
-  <si>
-    <t>somebody restart worst unable august getting cache response wait provide relogin services app another elses still im login solution call etc use doesnt banking customer 2018 clear work care asked asking dbs calls random phone please</t>
-  </si>
-  <si>
-    <t>somebody restart worst unable august getting cache response wait provide relogin services  another elses still im login solution call etc use doesnt  customer 2018 clear work care asked asking  calls random phone please</t>
-  </si>
-  <si>
-    <t>Vinod sadu</t>
-  </si>
-  <si>
-    <t>one care bank users proper u dont dbs know response cant customer neft send imps biggest restricting</t>
-  </si>
-  <si>
-    <t>one care  users proper u dont  know response cant customer neft send imps biggest restricting</t>
-  </si>
-  <si>
-    <t>abhilash pk</t>
-  </si>
-  <si>
-    <t>patience slow lot use need app come also cant log</t>
-  </si>
-  <si>
-    <t>patience slow lot use need  come also cant log</t>
-  </si>
-  <si>
-    <t>5 March 2019</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>best online processes application thing app little banking whole bit slower considered good thank goo</t>
-  </si>
-  <si>
-    <t>best online processes application thing  little  whole bit slower considered good thank goo</t>
-  </si>
-  <si>
-    <t>Venkateshan Mohan</t>
-  </si>
-  <si>
-    <t>permission work reason reasons rival enough call storage sms need getting without permissions banking security think phone os apps</t>
-  </si>
-  <si>
-    <t>permission work reason reasons rival enough call storage sms need getting without permissions  security think phone os apps</t>
-  </si>
-  <si>
-    <t>Madhu Gana</t>
-  </si>
-  <si>
-    <t>showing installed incorrect fix let 4 check reset problem months details app lost bought past digibank login password know responding mobile using properly new going please</t>
-  </si>
-  <si>
-    <t>showing installed incorrect fix let 4 check reset problem months details  lost bought past  login password know responding mobile using properly new going please</t>
-  </si>
-  <si>
-    <t>mahesh raut</t>
-  </si>
-  <si>
-    <t>trasted person month accounti acno wrong reason balance open account show digibank six password froud dont 43141 time ago every dedit please</t>
-  </si>
-  <si>
-    <t>trasted person month accounti acno wrong reason balance open account show  six password froud dont 43141 time ago every dedit please</t>
-  </si>
-  <si>
-    <t>waiting thanks bank crowd control thing dbs home everything</t>
-  </si>
-  <si>
-    <t>waiting thanks  crowd control thing  home everything</t>
-  </si>
-  <si>
-    <t>kamal kishor Joshi</t>
-  </si>
-  <si>
-    <t>contact way shows open app technical case able error digibank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact way shows open  technical case able error </t>
-  </si>
-  <si>
-    <t>date kyc complete mail bank city way aurangabad sugget dbs day within branch kindly right receive 90 got reply near</t>
-  </si>
-  <si>
-    <t>date kyc complete mail  city way aurangabad sugget  day within branch kindly right receive 90 got reply near</t>
-  </si>
-  <si>
-    <t>Vaithees Waran</t>
-  </si>
-  <si>
-    <t>option solve pin month also soon got issue kind times sort zeroi im pinafter save update monthly keypad chennaiplease card lot use possible result n work enter last activate try came debit trying</t>
-  </si>
-  <si>
-    <t>annoying facing problems account opened</t>
-  </si>
-  <si>
-    <t>suresh dongale</t>
-  </si>
-  <si>
-    <t>mobile thanks bank use application experience last dbs banking two well years</t>
-  </si>
-  <si>
-    <t>mobile thanks  use application experience last   two well years</t>
-  </si>
-  <si>
-    <t>Manish Kumar</t>
-  </si>
-  <si>
-    <t>bt disburse taking unale time personal server trying actionalays</t>
-  </si>
-  <si>
-    <t>slow never card worst app activate life seen received debit till able</t>
-  </si>
-  <si>
-    <t>slow never card worst  activate life seen received debit till able</t>
-  </si>
-  <si>
-    <t>Pramoda K S</t>
-  </si>
-  <si>
-    <t>money using recommend helps nice instant fixed application experience dbs 2 deposit within one transfer im since many years digibank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">money using recommend helps nice instant fixed application experience  2 deposit within one transfer im since many years </t>
-  </si>
-  <si>
-    <t>Rudransh Kumar</t>
-  </si>
-  <si>
-    <t>money whenever saying went always working something want transfer wrong</t>
-  </si>
-  <si>
-    <t>Black Hammer</t>
-  </si>
-  <si>
-    <t>resolved small town hope bank application still office app lagging also bit increase soon good service please</t>
-  </si>
-  <si>
-    <t>resolved small town hope  application still office  lagging also bit increase soon good service please</t>
-  </si>
-  <si>
-    <t>Himanshu Phulara</t>
-  </si>
-  <si>
-    <t>digibank credit card unable app make ro bill payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> credit card unable  make ro bill payment</t>
-  </si>
-  <si>
-    <t>Bijoy Rauth</t>
-  </si>
-  <si>
-    <t>applied days id tracking 2 received didnt first</t>
-  </si>
-  <si>
-    <t>penikalapati praveen</t>
-  </si>
-  <si>
-    <t>loans provide worst app quay throughout mention india</t>
-  </si>
-  <si>
-    <t>loans provide worst  quay throughout mention india</t>
-  </si>
-  <si>
-    <t>Pradyumna Kumar Sahoo</t>
-  </si>
-  <si>
-    <t>solution solves bank loved tips problems hassle seconds banking free digibot within finger</t>
-  </si>
-  <si>
-    <t>solution solves  loved tips problems hassle seconds  free digibot within finger</t>
-  </si>
-  <si>
-    <t>Suraj Avatade</t>
-  </si>
-  <si>
-    <t>money useless add option upi 3month bad card experience last debit want</t>
-  </si>
-  <si>
-    <t>Monika Arora</t>
-  </si>
-  <si>
-    <t>facing issue slow times app tech</t>
-  </si>
-  <si>
-    <t>facing issue slow times  tech</t>
-  </si>
-  <si>
-    <t>cash sachin adding amazing convenient withdrawals ambassador brand app tendulkar banking also transfer fund well 0 mr</t>
-  </si>
-  <si>
-    <t>cash sachin adding amazing convenient withdrawals ambassador brand  tendulkar  also transfer fund well 0 mr</t>
-  </si>
-  <si>
-    <t>Ajay Dubey</t>
-  </si>
-  <si>
-    <t>upi resolve issue dormant getting inactive account service</t>
-  </si>
-  <si>
-    <t>Sumit Jha</t>
-  </si>
-  <si>
-    <t>facing appany slow problems problem app time types regarding please solve process</t>
-  </si>
-  <si>
-    <t>facing appany slow problems problem  time types regarding please solve process</t>
-  </si>
-  <si>
-    <t>get digi bank card debit able</t>
-  </si>
-  <si>
-    <t>get digi  card debit able</t>
-  </si>
-  <si>
-    <t>Prem Dangat</t>
-  </si>
-  <si>
-    <t>customerthey u worst take service first offer digi download nd app r call sending eligible bankdont dont poor care making year appthey customer fool confirm</t>
-  </si>
-  <si>
-    <t>customerthey u worst take service first offer digi download nd  r call sending eligible bankdont dont poor care making year appthey customer fool confirm</t>
-  </si>
-  <si>
-    <t>Mahish Singh</t>
-  </si>
-  <si>
-    <t>registered person number working get called app lost someone applied anyone update neither call days says 2 verification arrival mobile aadar week customer</t>
-  </si>
-  <si>
-    <t>registered person number working get called  lost someone applied anyone update neither call days says 2 verification arrival mobile aadar week customer</t>
-  </si>
-  <si>
-    <t>Pahen Phom</t>
-  </si>
-  <si>
-    <t>get expecting daily wanna card extend temporarily complaints limit debit till good im</t>
-  </si>
-  <si>
-    <t>RAHUL RANJAN</t>
-  </si>
-  <si>
-    <t>get problem doesnt always otp probably servers</t>
-  </si>
-  <si>
-    <t>B C</t>
-  </si>
-  <si>
-    <t>sing waste match password id app wasted totally poor working tried time username correct</t>
-  </si>
-  <si>
-    <t>sing waste match password id  wasted totally poor working tried time username correct</t>
-  </si>
-  <si>
-    <t>options deposits completely upi charges much faq bank fixed better withdrawals cons program also pros good offers apps great atms would scorecard app account digibot checked digibucks bill savings etc card finally aside dont robust pay banking integrate therein accounts help digital atm include dbs payments debit many</t>
-  </si>
-  <si>
-    <t>options deposits completely upi charges much faq  fixed better withdrawals cons program also pros good offers apps great atms would scorecard  account digibot checked digibucks bill savings etc card finally aside dont robust pay  integrate therein accounts help digital atm include  payments debit many</t>
-  </si>
-  <si>
-    <t>Prashant Kumar</t>
-  </si>
-  <si>
-    <t>useless hang maximum application app time crease going service</t>
-  </si>
-  <si>
-    <t>useless hang maximum application  time crease going service</t>
-  </si>
-  <si>
-    <t>Ali Ajmeri</t>
-  </si>
-  <si>
-    <t>slow problems app kindly still speed</t>
-  </si>
-  <si>
-    <t>slow problems  kindly still speed</t>
-  </si>
-  <si>
-    <t>sajid rabi</t>
-  </si>
-  <si>
-    <t>improvement plz se apps hota atm koi nai kai camplain kiya bhi withdrawal horah transfer recharge help fashi payment na</t>
-  </si>
-  <si>
-    <t>Soumik Naskar</t>
-  </si>
-  <si>
-    <t>dbs good uperb app</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> good uperb </t>
-  </si>
-  <si>
-    <t>Sita Rama Reddy Burramukku</t>
-  </si>
-  <si>
-    <t>ifs money code add wallet resolve unable even number ac correct though first given</t>
-  </si>
-  <si>
-    <t>Anand Singh</t>
-  </si>
-  <si>
-    <t>exit using back app button able</t>
-  </si>
-  <si>
-    <t>exit using back  button able</t>
-  </si>
-  <si>
-    <t>NEERA MANKAD</t>
-  </si>
-  <si>
-    <t>best wallet proud bank use funds worlds app account providing safest ane one user friendly intrest</t>
-  </si>
-  <si>
-    <t>best wallet proud  use funds worlds  account providing safest ane one user friendly intrest</t>
-  </si>
-  <si>
-    <t>Manoj Pandey</t>
-  </si>
-  <si>
-    <t>best one bank use app account banking salary come benefits acrosscan</t>
-  </si>
-  <si>
-    <t>best one  use  account  salary come benefits acrosscan</t>
-  </si>
-  <si>
-    <t>Mohammed Iftekhar Aalam</t>
-  </si>
-  <si>
-    <t>password reset forgotten unable</t>
-  </si>
-  <si>
-    <t>ramesh babu</t>
-  </si>
-  <si>
-    <t>best excellent team use times dbs app easy system banking service lagging</t>
-  </si>
-  <si>
-    <t>best excellent team use times   easy system  service lagging</t>
-  </si>
-  <si>
-    <t>Gourab Das</t>
-  </si>
-  <si>
-    <t>charges maintenance fingertips atm amt use cool without easy become min well</t>
-  </si>
-  <si>
-    <t>A M</t>
-  </si>
-  <si>
-    <t>stop slow banking bit one</t>
-  </si>
-  <si>
-    <t>stop slow  bit one</t>
-  </si>
-  <si>
-    <t>Ujjwal Sancheti</t>
-  </si>
-  <si>
-    <t>provide card provided days number tracking working received 2 next guaranteed 3</t>
-  </si>
-  <si>
-    <t>blue worst dart customer service</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>best digital bank experience app usage account opening truly anything awesome seamless</t>
-  </si>
-  <si>
-    <t>best digital  experience  usage account opening truly anything awesome seamless</t>
-  </si>
-  <si>
-    <t>B N Mahanta</t>
-  </si>
-  <si>
-    <t>saving odishait bad use open experience app easy account able good</t>
-  </si>
-  <si>
-    <t>saving odishait bad use open experience  easy account able good</t>
-  </si>
-  <si>
-    <t>Samir Nayakawadi</t>
-  </si>
-  <si>
-    <t>option virtual card would like rest app debit things awesome</t>
-  </si>
-  <si>
-    <t>option virtual card would like rest  debit things awesome</t>
-  </si>
-  <si>
-    <t>Yuvaraj Desav</t>
-  </si>
-  <si>
-    <t>best work branches excited job bank use lot must app dbs interested</t>
-  </si>
-  <si>
-    <t>best work branches excited job  use lot must   interested</t>
-  </si>
-  <si>
-    <t>HITESH VEER</t>
-  </si>
-  <si>
-    <t>care mumbai number fast branch customer please reply found</t>
-  </si>
-  <si>
-    <t>atm withdrawal happy limitation</t>
-  </si>
-  <si>
-    <t>Partha Hudati</t>
-  </si>
-  <si>
-    <t>start improvement star lot still need giving done one thats 3</t>
-  </si>
-  <si>
-    <t>shivam singh</t>
-  </si>
-  <si>
-    <t>login back version previous even app account cant restore please</t>
-  </si>
-  <si>
-    <t>login back version previous even  account cant restore please</t>
-  </si>
-  <si>
-    <t>Shivkumar Ladde</t>
-  </si>
-  <si>
-    <t>person easy normal good operate</t>
-  </si>
-  <si>
-    <t>Shubham Bakal</t>
-  </si>
-  <si>
-    <t>made perfect much live bank less sense respect dbs easy banking makes love lots india digibank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">made perfect much live  less sense respect  easy  makes love lots india </t>
-  </si>
-  <si>
-    <t>Bharat Gunjawate</t>
-  </si>
-  <si>
-    <t>money suggestion add option nice card use every app make available debit one</t>
-  </si>
-  <si>
-    <t>money suggestion add option nice card use every  make available debit one</t>
-  </si>
-  <si>
-    <t>Harshit Gupta</t>
-  </si>
-  <si>
-    <t>much good times even 23 appsits slow compared internet banking connectionthe verification smooth process works timeits buffering shows takes buffer always lags fails</t>
-  </si>
-  <si>
-    <t>much good times even 23 appsits slow compared internet  connectionthe verification smooth process works timeits buffering shows takes buffer always lags fails</t>
+    <t>puas bank cicilan kabur jawafull yg tidak chat pihak diberikan jawaban tanpa dengan bayar hubungi selesai tapi bunga utk blm apakah namanya keluarnya full live atau minimum duluan sangat akan transaksi bertanggung kena menyatakan solusi menanyakan review dorisbuda</t>
+  </si>
+  <si>
+    <t>Indra Utama</t>
+  </si>
+  <si>
+    <t>tokopedia bank problem android pake msh selalu regis baru ngaco akun simple irritating semoga error coba s7 berhasil setelah tgl berikutnya di terpaksa server 6 review update full skrg versi website per apps karena lewat dan rating 2019 pun saya terupdate maret melalui samsung</t>
+  </si>
+  <si>
+    <t>tokopedia bank problem android pake msh selalu regis baru ngaco akun simple irritating semoga error coba s7 berhasil setelah tgl berikutnya di terpaksa server 6 review update full skrg versi website per  karena lewat dan rating 2019 pun saya terupdate maret melalui samsung</t>
+  </si>
+  <si>
+    <t>sekar utamie</t>
+  </si>
+  <si>
+    <t>baik2 diperbaiki segera terus toped cepat loading padahal setelah untuk saja tolong malahan sebelum jd perhitungan ga force update versi yah stop thanks lambat kok nya belanjaan dan pernah lama</t>
+  </si>
+  <si>
+    <t>tokopedia hp dari selang baru tidak ngelag app setelah keluar tokopedianya tapi harus klik fix 10menit responding lagi seperti gak full dibuka langsung ikon setiap ngapangapain dan semula bisa direstart review</t>
+  </si>
+  <si>
+    <t>tokopedia hp dari selang baru tidak ngelag  setelah keluar tokopedianya tapi harus klik fix 10menit responding lagi seperti gak full dibuka langsung ikon setiap ngapangapain dan semula bisa direstart review</t>
+  </si>
+  <si>
+    <t>Bangun Sucipto</t>
+  </si>
+  <si>
+    <t>ilang bayarpake gosend minggu jg sampeseller stts dah sampe2 barang malem ga pesen tp update responbilang sampe instan kurir senin slow orderan hari kaga dikirim parahduit</t>
+  </si>
+  <si>
+    <t>Ali Nurzaman</t>
+  </si>
+  <si>
+    <t>apalagi doang tokopedia ratingnya pake teramafull ini memberi tidak penjual kalau selektif tolong maaf nama di seperti loh sayang spam yang ada percuma besar nya dan masalah cs ngasih saya terhadap karna turunkan solusi cuman review lebih menyelesikan</t>
+  </si>
+  <si>
+    <t>Vincentius Fo KingHo</t>
+  </si>
+  <si>
+    <t>tokopedia pada pake selalu sejak wifi diskusi coba padahal depan kesalahan halaman terjadi ga sekali server update terbaru juga dan aja pembelian bisa cuma akses sama dll data</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>pake akun caranya customer dijelasin punya luculucuuuuuumasa melanggar tapi respect barang gitudibilang ga mau gak bgtga supportnyacurang hahahhaa dibilang kenapa beli promo bgt pernah bisa 2 buat sama</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1046,7 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1147,25 +1054,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1173,25 +1080,25 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1199,25 +1106,25 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1225,25 +1132,25 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1251,25 +1158,25 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1277,25 +1184,25 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1303,25 +1210,25 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1329,25 +1236,25 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1355,25 +1262,25 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1381,25 +1288,25 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="s">
         <v>48</v>
-      </c>
-      <c r="G14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1407,25 +1314,25 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1433,25 +1340,25 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" t="s">
         <v>48</v>
-      </c>
-      <c r="G16" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1459,25 +1366,25 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1485,77 +1392,73 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" t="s">
-        <v>73</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H18" t="s"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="n">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" t="s">
-        <v>77</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H19" t="s"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="n">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1563,25 +1466,25 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1589,25 +1492,25 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1615,10 +1518,10 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -1627,13 +1530,13 @@
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1641,25 +1544,25 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="G24" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1667,25 +1570,25 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="H25" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1693,25 +1596,25 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
         <v>28</v>
       </c>
-      <c r="D26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" t="s">
-        <v>48</v>
-      </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="G26" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="H26" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1719,25 +1622,25 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="G27" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1745,25 +1648,25 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="G28" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1771,25 +1674,25 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" t="s">
         <v>22</v>
       </c>
-      <c r="E29" t="s">
-        <v>23</v>
-      </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="G29" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="H29" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1797,25 +1700,25 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="G30" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="H30" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1823,25 +1726,25 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="G31" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="H31" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1849,25 +1752,25 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="G32" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="H32" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1875,25 +1778,25 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G33" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="H33" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1901,25 +1804,25 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="G34" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="H34" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1927,25 +1830,25 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G35" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="H35" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1953,25 +1856,25 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="G36" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="H36" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1979,25 +1882,25 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="G37" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="H37" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2005,25 +1908,25 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="H38" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2031,25 +1934,25 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="H39" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2057,25 +1960,25 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F40" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="H40" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2083,25 +1986,25 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="H41" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2109,25 +2012,25 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="G42" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="H42" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2135,25 +2038,25 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G43" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="H43" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2161,25 +2064,25 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="H44" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2187,25 +2090,25 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G45" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="H45" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2213,25 +2116,25 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="G46" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="H46" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2239,25 +2142,25 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>148</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="D47" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F47" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G47" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="H47" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2265,25 +2168,25 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F48" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G48" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="H48" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2291,25 +2194,25 @@
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G49" t="s">
-        <v>153</v>
+        <v>47</v>
       </c>
       <c r="H49" t="s">
-        <v>154</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2317,25 +2220,25 @@
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" t="s">
+        <v>135</v>
+      </c>
+      <c r="H50" t="s">
         <v>48</v>
-      </c>
-      <c r="F50" t="s">
-        <v>55</v>
-      </c>
-      <c r="G50" t="s">
-        <v>156</v>
-      </c>
-      <c r="H50" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2343,25 +2246,25 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F51" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G51" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="H51" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2369,25 +2272,25 @@
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D52" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F52" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G52" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="H52" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2395,51 +2298,49 @@
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F53" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G53" t="s">
-        <v>164</v>
-      </c>
-      <c r="H53" t="s">
-        <v>164</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="H53" t="s"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="n">
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="E54" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F54" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G54" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="H54" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2447,25 +2348,25 @@
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="C55" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="E55" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F55" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G55" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
       <c r="H55" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2473,25 +2374,25 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G56" t="s">
-        <v>171</v>
+        <v>47</v>
       </c>
       <c r="H56" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2499,103 +2400,97 @@
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F57" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G57" t="s">
-        <v>174</v>
-      </c>
-      <c r="H57" t="s">
-        <v>175</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H57" t="s"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="n">
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D58" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E58" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="F58" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G58" t="s">
-        <v>177</v>
-      </c>
-      <c r="H58" t="s">
-        <v>177</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H58" t="s"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="n">
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="D59" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F59" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="G59" t="s">
-        <v>179</v>
-      </c>
-      <c r="H59" t="s">
-        <v>180</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H59" t="s"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="n">
         <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E60" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F60" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G60" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="H60" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2603,25 +2498,25 @@
         <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>27</v>
       </c>
       <c r="C61" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G61" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="H61" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2629,25 +2524,25 @@
         <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="D62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" t="s">
         <v>22</v>
       </c>
-      <c r="E62" t="s">
-        <v>23</v>
-      </c>
       <c r="F62" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="G62" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="H62" t="s">
-        <v>188</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2655,25 +2550,25 @@
         <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="C63" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E63" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>161</v>
       </c>
       <c r="G63" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="H63" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2681,25 +2576,25 @@
         <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D64" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="E64" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F64" t="s">
-        <v>55</v>
+        <v>164</v>
       </c>
       <c r="G64" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="H64" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2707,25 +2602,25 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="C65" t="s">
         <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="E65" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F65" t="s">
-        <v>55</v>
+        <v>167</v>
       </c>
       <c r="G65" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="H65" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2733,25 +2628,25 @@
         <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="C66" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E66" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F66" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G66" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="H66" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2759,25 +2654,25 @@
         <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E67" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>55</v>
+        <v>174</v>
       </c>
       <c r="G67" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="H67" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2785,25 +2680,25 @@
         <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>202</v>
+        <v>27</v>
       </c>
       <c r="C68" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="D68" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="E68" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F68" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G68" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="H68" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2811,25 +2706,25 @@
         <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D69" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F69" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G69" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="H69" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2837,25 +2732,25 @@
         <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>179</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="D70" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F70" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="G70" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="H70" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2863,25 +2758,25 @@
         <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="C71" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="E71" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F71" t="s">
-        <v>55</v>
+        <v>167</v>
       </c>
       <c r="G71" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="H71" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2889,25 +2784,25 @@
         <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="C72" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D72" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E72" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F72" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G72" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="H72" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2915,25 +2810,25 @@
         <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="C73" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D73" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E73" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F73" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="G73" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="H73" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2941,25 +2836,25 @@
         <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C74" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="D74" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E74" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="F74" t="s">
-        <v>55</v>
+        <v>188</v>
       </c>
       <c r="G74" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="H74" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2967,25 +2862,25 @@
         <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>50</v>
+        <v>190</v>
       </c>
       <c r="C75" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D75" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="E75" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F75" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G75" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="H75" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2993,25 +2888,25 @@
         <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D76" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E76" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F76" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="H76" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3019,25 +2914,25 @@
         <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>222</v>
+        <v>27</v>
       </c>
       <c r="C77" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D77" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E77" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F77" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G77" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="H77" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3045,25 +2940,25 @@
         <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="C78" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D78" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E78" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F78" t="s">
         <v>10</v>
       </c>
       <c r="G78" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="H78" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3071,25 +2966,25 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="C79" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D79" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E79" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F79" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="G79" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="H79" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3097,25 +2992,25 @@
         <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="C80" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D80" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E80" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F80" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G80" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="H80" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3123,25 +3018,25 @@
         <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="C81" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G81" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="H81" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>